<commit_message>
Created my own SumOfAllDisease column
</commit_message>
<xml_diff>
--- a/SCTLD_Annual_Summaries.xlsx
+++ b/SCTLD_Annual_Summaries.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Counts_SCTLD</t>
   </si>
   <si>
-    <t xml:space="preserve">Counts_AnyDisease</t>
+    <t xml:space="preserve">Counts_AllDisease</t>
   </si>
   <si>
     <t xml:space="preserve">Total_Coral_Counts</t>
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>421</v>
@@ -453,7 +453,7 @@
         <v>0.475059382422803</v>
       </c>
       <c r="F3" t="n">
-        <v>0.475059382422803</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
         <v>460</v>
@@ -473,7 +473,7 @@
         <v>0.869565217391304</v>
       </c>
       <c r="F4" t="n">
-        <v>1.52173913043478</v>
+        <v>0.652173913043478</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>398</v>
@@ -493,7 +493,7 @@
         <v>3.01507537688442</v>
       </c>
       <c r="F5" t="n">
-        <v>3.51758793969849</v>
+        <v>0.50251256281407</v>
       </c>
     </row>
     <row r="6">
@@ -504,7 +504,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>223</v>
@@ -513,7 +513,7 @@
         <v>16.1434977578475</v>
       </c>
       <c r="F6" t="n">
-        <v>16.5919282511211</v>
+        <v>0.896860986547085</v>
       </c>
     </row>
     <row r="7">
@@ -524,7 +524,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>201</v>
@@ -533,7 +533,7 @@
         <v>7.46268656716418</v>
       </c>
       <c r="F7" t="n">
-        <v>7.96019900497512</v>
+        <v>0.497512437810945</v>
       </c>
     </row>
     <row r="8">
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>225</v>
@@ -553,7 +553,7 @@
         <v>5.33333333333333</v>
       </c>
       <c r="F8" t="n">
-        <v>5.33333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -564,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>245</v>
@@ -573,7 +573,7 @@
         <v>2.44897959183673</v>
       </c>
       <c r="F9" t="n">
-        <v>2.44897959183673</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>263</v>
@@ -593,7 +593,7 @@
         <v>0.380228136882129</v>
       </c>
       <c r="F10" t="n">
-        <v>0.380228136882129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>257</v>
@@ -613,7 +613,7 @@
         <v>0.389105058365759</v>
       </c>
       <c r="F11" t="n">
-        <v>0.389105058365759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>296</v>
@@ -633,7 +633,7 @@
         <v>0.675675675675676</v>
       </c>
       <c r="F12" t="n">
-        <v>0.675675675675676</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>331</v>
@@ -653,7 +653,7 @@
         <v>0.906344410876133</v>
       </c>
       <c r="F13" t="n">
-        <v>0.906344410876133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -664,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>371</v>
@@ -673,7 +673,7 @@
         <v>1.07816711590297</v>
       </c>
       <c r="F14" t="n">
-        <v>1.07816711590297</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>58</v>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.72413793103448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -862,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>45</v>
@@ -871,7 +871,7 @@
         <v>4.44444444444444</v>
       </c>
       <c r="G8" t="n">
-        <v>4.44444444444444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>41</v>
@@ -894,7 +894,7 @@
         <v>2.4390243902439</v>
       </c>
       <c r="G9" t="n">
-        <v>2.4390243902439</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -931,7 +931,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>32</v>
@@ -940,7 +940,7 @@
         <v>12.5</v>
       </c>
       <c r="G11" t="n">
-        <v>12.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>601</v>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.66389351081531</v>
+        <v>0.998336106489185</v>
       </c>
     </row>
     <row r="3">
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>533</v>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.68855534709193</v>
+        <v>0.562851782363977</v>
       </c>
     </row>
     <row r="4">
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
         <v>516</v>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>3.10077519379845</v>
+        <v>0.968992248062015</v>
       </c>
     </row>
     <row r="5">
@@ -1129,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>500</v>
@@ -1138,7 +1138,7 @@
         <v>0.4</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1152,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>501</v>
@@ -1161,7 +1161,7 @@
         <v>0.598802395209581</v>
       </c>
       <c r="G6" t="n">
-        <v>3.59281437125748</v>
+        <v>0.798403193612774</v>
       </c>
     </row>
     <row r="7">
@@ -1175,7 +1175,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
         <v>449</v>
@@ -1184,7 +1184,7 @@
         <v>4.23162583518931</v>
       </c>
       <c r="G7" t="n">
-        <v>6.23608017817372</v>
+        <v>0.89086859688196</v>
       </c>
     </row>
     <row r="8">
@@ -1198,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
         <v>443</v>
@@ -1207,7 +1207,7 @@
         <v>3.83747178329571</v>
       </c>
       <c r="G8" t="n">
-        <v>9.48081264108352</v>
+        <v>0.677200902934537</v>
       </c>
     </row>
     <row r="9">
@@ -1221,7 +1221,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
         <v>421</v>
@@ -1230,7 +1230,7 @@
         <v>5.46318289786223</v>
       </c>
       <c r="G9" t="n">
-        <v>5.93824228028503</v>
+        <v>0.950118764845606</v>
       </c>
     </row>
     <row r="10">
@@ -1244,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>383</v>
@@ -1253,7 +1253,7 @@
         <v>1.56657963446475</v>
       </c>
       <c r="G10" t="n">
-        <v>3.1331592689295</v>
+        <v>0.522193211488251</v>
       </c>
     </row>
     <row r="11">
@@ -1267,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>372</v>
@@ -1276,7 +1276,7 @@
         <v>4.03225806451613</v>
       </c>
       <c r="G11" t="n">
-        <v>4.3010752688172</v>
+        <v>0.537634408602151</v>
       </c>
     </row>
     <row r="12">
@@ -1290,7 +1290,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="n">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
         <v>334</v>
@@ -1299,7 +1299,7 @@
         <v>19.4610778443114</v>
       </c>
       <c r="G12" t="n">
-        <v>20.9580838323353</v>
+        <v>0.598802395209581</v>
       </c>
     </row>
     <row r="13">
@@ -1313,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E13" t="n">
         <v>282</v>
@@ -1322,7 +1322,7 @@
         <v>3.90070921985816</v>
       </c>
       <c r="G13" t="n">
-        <v>4.60992907801418</v>
+        <v>0.709219858156028</v>
       </c>
     </row>
     <row r="14">
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>269</v>
@@ -1345,7 +1345,7 @@
         <v>0.371747211895911</v>
       </c>
       <c r="G14" t="n">
-        <v>0.371747211895911</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>84</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.19047619047619</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>93</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2.1505376344086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>95</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.05263157894737</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>96</v>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>3.125</v>
+        <v>1.04166666666667</v>
       </c>
     </row>
     <row r="7">
@@ -1511,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>89</v>
@@ -1520,7 +1520,7 @@
         <v>3.37078651685393</v>
       </c>
       <c r="G7" t="n">
-        <v>3.37078651685393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1534,7 +1534,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>66</v>
@@ -1543,7 +1543,7 @@
         <v>3.03030303030303</v>
       </c>
       <c r="G8" t="n">
-        <v>3.03030303030303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>58</v>
@@ -1566,7 +1566,7 @@
         <v>1.72413793103448</v>
       </c>
       <c r="G9" t="n">
-        <v>1.72413793103448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>56</v>
@@ -1612,7 +1612,7 @@
         <v>3.57142857142857</v>
       </c>
       <c r="G11" t="n">
-        <v>3.57142857142857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>34</v>
@@ -1635,7 +1635,7 @@
         <v>2.94117647058824</v>
       </c>
       <c r="G12" t="n">
-        <v>2.94117647058824</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>235</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2.12765957446809</v>
+        <v>1.70212765957447</v>
       </c>
     </row>
     <row r="3">
@@ -1826,7 +1826,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>152</v>
@@ -1835,7 +1835,7 @@
         <v>19.0789473684211</v>
       </c>
       <c r="F7" t="n">
-        <v>19.7368421052632</v>
+        <v>2.63157894736842</v>
       </c>
     </row>
     <row r="8">
@@ -1846,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>104</v>
@@ -1855,7 +1855,7 @@
         <v>9.61538461538462</v>
       </c>
       <c r="F8" t="n">
-        <v>9.61538461538462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1866,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>109</v>
@@ -1875,7 +1875,7 @@
         <v>2.75229357798165</v>
       </c>
       <c r="F9" t="n">
-        <v>2.75229357798165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2120,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>477</v>
@@ -2129,7 +2129,7 @@
         <v>0.419287211740042</v>
       </c>
       <c r="F7" t="n">
-        <v>0.628930817610063</v>
+        <v>0.209643605870021</v>
       </c>
     </row>
     <row r="8">
@@ -2140,7 +2140,7 @@
         <v>95</v>
       </c>
       <c r="C8" t="n">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>332</v>
@@ -2149,7 +2149,7 @@
         <v>28.6144578313253</v>
       </c>
       <c r="F8" t="n">
-        <v>28.6144578313253</v>
+        <v>0.602409638554217</v>
       </c>
     </row>
     <row r="9">
@@ -2160,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>303</v>
@@ -2169,7 +2169,7 @@
         <v>2.64026402640264</v>
       </c>
       <c r="F9" t="n">
-        <v>2.64026402640264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2180,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>258</v>
@@ -2189,7 +2189,7 @@
         <v>0.387596899224806</v>
       </c>
       <c r="F10" t="n">
-        <v>0.387596899224806</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2200,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>269</v>
@@ -2209,7 +2209,7 @@
         <v>4.08921933085502</v>
       </c>
       <c r="F11" t="n">
-        <v>4.08921933085502</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2220,7 +2220,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>273</v>
@@ -2229,7 +2229,7 @@
         <v>2.93040293040293</v>
       </c>
       <c r="F12" t="n">
-        <v>3.2967032967033</v>
+        <v>0.366300366300366</v>
       </c>
     </row>
     <row r="13">
@@ -2240,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>261</v>
@@ -2249,7 +2249,7 @@
         <v>1.53256704980843</v>
       </c>
       <c r="F13" t="n">
-        <v>1.53256704980843</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="n">
         <v>747</v>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.803212851405622</v>
+        <v>0.937081659973226</v>
       </c>
     </row>
     <row r="7">
@@ -2434,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>678</v>
@@ -2443,7 +2443,7 @@
         <v>1.47492625368732</v>
       </c>
       <c r="F8" t="n">
-        <v>1.76991150442478</v>
+        <v>0.294985250737463</v>
       </c>
     </row>
     <row r="9">
@@ -2454,7 +2454,7 @@
         <v>58</v>
       </c>
       <c r="C9" t="n">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
         <v>589</v>
@@ -2463,7 +2463,7 @@
         <v>9.8471986417657</v>
       </c>
       <c r="F9" t="n">
-        <v>9.8471986417657</v>
+        <v>0.169779286926995</v>
       </c>
     </row>
     <row r="10">
@@ -2474,7 +2474,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>379</v>
@@ -2483,7 +2483,7 @@
         <v>3.43007915567282</v>
       </c>
       <c r="F10" t="n">
-        <v>3.69393139841689</v>
+        <v>0.263852242744063</v>
       </c>
     </row>
     <row r="11">
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
         <v>372</v>
@@ -2503,7 +2503,7 @@
         <v>5.91397849462366</v>
       </c>
       <c r="F11" t="n">
-        <v>6.45161290322581</v>
+        <v>0.806451612903226</v>
       </c>
     </row>
     <row r="12">
@@ -2514,7 +2514,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>365</v>
@@ -2523,7 +2523,7 @@
         <v>1.64383561643836</v>
       </c>
       <c r="F12" t="n">
-        <v>1.91780821917808</v>
+        <v>0.273972602739726</v>
       </c>
     </row>
     <row r="13">
@@ -2534,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>355</v>
@@ -2543,7 +2543,7 @@
         <v>0.845070422535211</v>
       </c>
       <c r="F13" t="n">
-        <v>1.12676056338028</v>
+        <v>0.28169014084507</v>
       </c>
     </row>
     <row r="14">
@@ -2608,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>619</v>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.13085621970921</v>
+        <v>0.969305331179321</v>
       </c>
     </row>
     <row r="3">
@@ -2788,7 +2788,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>465</v>
@@ -2797,7 +2797,7 @@
         <v>4.51612903225806</v>
       </c>
       <c r="F11" t="n">
-        <v>4.73118279569892</v>
+        <v>0.21505376344086</v>
       </c>
     </row>
     <row r="12">
@@ -2808,7 +2808,7 @@
         <v>108</v>
       </c>
       <c r="C12" t="n">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
         <v>277</v>
@@ -2817,7 +2817,7 @@
         <v>38.9891696750903</v>
       </c>
       <c r="F12" t="n">
-        <v>39.3501805054152</v>
+        <v>0.36101083032491</v>
       </c>
     </row>
     <row r="13">
@@ -2828,7 +2828,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>205</v>
@@ -2837,7 +2837,7 @@
         <v>7.31707317073171</v>
       </c>
       <c r="F13" t="n">
-        <v>7.80487804878049</v>
+        <v>0.48780487804878</v>
       </c>
     </row>
     <row r="14">
@@ -2848,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>208</v>
@@ -2857,7 +2857,7 @@
         <v>0.961538461538462</v>
       </c>
       <c r="F14" t="n">
-        <v>0.961538461538462</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2908,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>222</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.45045045045045</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2931,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>229</v>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.74672489082969</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>289</v>
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.3840830449827</v>
+        <v>1.03806228373702</v>
       </c>
     </row>
     <row r="5">
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>249</v>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.803212851405622</v>
+        <v>0.401606425702811</v>
       </c>
     </row>
     <row r="7">
@@ -3023,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>251</v>
@@ -3032,7 +3032,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="G7" t="n">
-        <v>0.796812749003984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -3046,7 +3046,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>190</v>
@@ -3055,7 +3055,7 @@
         <v>15.2631578947368</v>
       </c>
       <c r="G8" t="n">
-        <v>16.8421052631579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>156</v>
@@ -3078,7 +3078,7 @@
         <v>6.41025641025641</v>
       </c>
       <c r="G9" t="n">
-        <v>6.41025641025641</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3092,7 +3092,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>93</v>
@@ -3101,7 +3101,7 @@
         <v>2.1505376344086</v>
       </c>
       <c r="G10" t="n">
-        <v>2.1505376344086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3115,7 +3115,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>87</v>
@@ -3124,7 +3124,7 @@
         <v>5.74712643678161</v>
       </c>
       <c r="G11" t="n">
-        <v>5.74712643678161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3138,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>64</v>
@@ -3147,7 +3147,7 @@
         <v>6.25</v>
       </c>
       <c r="G12" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -3359,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>49</v>
@@ -3368,7 +3368,7 @@
         <v>2.04081632653061</v>
       </c>
       <c r="G7" t="n">
-        <v>2.04081632653061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -3382,7 +3382,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>31</v>
@@ -3391,7 +3391,7 @@
         <v>16.1290322580645</v>
       </c>
       <c r="G8" t="n">
-        <v>16.1290322580645</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3405,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>25</v>
@@ -3414,7 +3414,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>26</v>
@@ -3460,7 +3460,7 @@
         <v>3.84615384615385</v>
       </c>
       <c r="G11" t="n">
-        <v>3.84615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3626,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
         <v>215</v>
@@ -3635,7 +3635,7 @@
         <v>0.930232558139535</v>
       </c>
       <c r="G4" t="n">
-        <v>3.25581395348837</v>
+        <v>2.7906976744186</v>
       </c>
     </row>
     <row r="5">
@@ -3649,7 +3649,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>208</v>
@@ -3658,7 +3658,7 @@
         <v>2.40384615384615</v>
       </c>
       <c r="G5" t="n">
-        <v>3.36538461538462</v>
+        <v>2.88461538461538</v>
       </c>
     </row>
     <row r="6">
@@ -3695,7 +3695,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>129</v>
@@ -3704,7 +3704,7 @@
         <v>2.32558139534884</v>
       </c>
       <c r="G7" t="n">
-        <v>2.32558139534884</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -3718,7 +3718,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>99</v>
@@ -3727,7 +3727,7 @@
         <v>15.1515151515152</v>
       </c>
       <c r="G8" t="n">
-        <v>16.1616161616162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3741,7 +3741,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>64</v>
@@ -3750,7 +3750,7 @@
         <v>3.125</v>
       </c>
       <c r="G9" t="n">
-        <v>3.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -3916,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>1073</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.745573159366263</v>
+        <v>0.65237651444548</v>
       </c>
     </row>
     <row r="3">
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
         <v>1123</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.534283170080142</v>
+        <v>0.267141585040071</v>
       </c>
     </row>
     <row r="4">
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
         <v>1163</v>
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.945829750644884</v>
+        <v>0.60189165950129</v>
       </c>
     </row>
     <row r="5">
@@ -4008,7 +4008,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E6" t="n">
         <v>1058</v>
@@ -4017,7 +4017,7 @@
         <v>3.11909262759924</v>
       </c>
       <c r="G6" t="n">
-        <v>4.06427221172023</v>
+        <v>3.40264650283554</v>
       </c>
     </row>
     <row r="7">
@@ -4031,7 +4031,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
         <v>993</v>
@@ -4040,7 +4040,7 @@
         <v>1.81268882175227</v>
       </c>
       <c r="G7" t="n">
-        <v>1.91339375629406</v>
+        <v>1.4098690835851</v>
       </c>
     </row>
     <row r="8">
@@ -4054,7 +4054,7 @@
         <v>57</v>
       </c>
       <c r="D8" t="n">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
         <v>988</v>
@@ -4063,7 +4063,7 @@
         <v>5.76923076923077</v>
       </c>
       <c r="G8" t="n">
-        <v>5.97165991902834</v>
+        <v>1.01214574898785</v>
       </c>
     </row>
     <row r="9">
@@ -4077,7 +4077,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="E9" t="n">
         <v>948</v>
@@ -4086,7 +4086,7 @@
         <v>3.69198312236287</v>
       </c>
       <c r="G9" t="n">
-        <v>3.69198312236287</v>
+        <v>0.527426160337553</v>
       </c>
     </row>
     <row r="10">
@@ -4100,7 +4100,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>854</v>
@@ -4109,7 +4109,7 @@
         <v>0.819672131147541</v>
       </c>
       <c r="G10" t="n">
-        <v>1.17096018735363</v>
+        <v>0.234192037470726</v>
       </c>
     </row>
     <row r="11">
@@ -4123,7 +4123,7 @@
         <v>28</v>
       </c>
       <c r="D11" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
         <v>875</v>
@@ -4132,7 +4132,7 @@
         <v>3.2</v>
       </c>
       <c r="G11" t="n">
-        <v>3.42857142857143</v>
+        <v>0.342857142857143</v>
       </c>
     </row>
     <row r="12">
@@ -4146,7 +4146,7 @@
         <v>54</v>
       </c>
       <c r="D12" t="n">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
         <v>800</v>
@@ -4155,7 +4155,7 @@
         <v>6.75</v>
       </c>
       <c r="G12" t="n">
-        <v>6.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13">
@@ -4169,7 +4169,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E13" t="n">
         <v>804</v>
@@ -4178,7 +4178,7 @@
         <v>1.74129353233831</v>
       </c>
       <c r="G13" t="n">
-        <v>1.74129353233831</v>
+        <v>0.373134328358209</v>
       </c>
     </row>
     <row r="14">
@@ -4192,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" t="n">
         <v>849</v>
@@ -4201,7 +4201,7 @@
         <v>0.588928150765607</v>
       </c>
       <c r="G14" t="n">
-        <v>0.706713780918728</v>
+        <v>0.588928150765607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SCTLD work with z_Colonies table
</commit_message>
<xml_diff>
--- a/SCTLD_Annual_Summaries.xlsx
+++ b/SCTLD_Annual_Summaries.xlsx
@@ -424,7 +424,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>262</v>
@@ -433,7 +433,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>0.381679389312977</v>
       </c>
     </row>
     <row r="3">
@@ -444,7 +444,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>421</v>
@@ -453,7 +453,7 @@
         <v>0.475059382422803</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.475059382422803</v>
       </c>
     </row>
     <row r="4">
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>460</v>
@@ -473,7 +473,7 @@
         <v>0.869565217391304</v>
       </c>
       <c r="F4" t="n">
-        <v>0.652173913043478</v>
+        <v>1.95652173913044</v>
       </c>
     </row>
     <row r="5">
@@ -484,7 +484,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
         <v>398</v>
@@ -493,7 +493,7 @@
         <v>3.01507537688442</v>
       </c>
       <c r="F5" t="n">
-        <v>0.50251256281407</v>
+        <v>3.76884422110553</v>
       </c>
     </row>
     <row r="6">
@@ -504,7 +504,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D6" t="n">
         <v>223</v>
@@ -513,7 +513,7 @@
         <v>16.1434977578475</v>
       </c>
       <c r="F6" t="n">
-        <v>0.896860986547085</v>
+        <v>17.4887892376682</v>
       </c>
     </row>
     <row r="7">
@@ -524,7 +524,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
         <v>201</v>
@@ -533,7 +533,7 @@
         <v>7.46268656716418</v>
       </c>
       <c r="F7" t="n">
-        <v>0.497512437810945</v>
+        <v>7.96019900497512</v>
       </c>
     </row>
     <row r="8">
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
         <v>225</v>
@@ -553,7 +553,7 @@
         <v>5.33333333333333</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>5.77777777777778</v>
       </c>
     </row>
     <row r="9">
@@ -564,7 +564,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D9" t="n">
         <v>245</v>
@@ -573,7 +573,7 @@
         <v>2.44897959183673</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>3.26530612244898</v>
       </c>
     </row>
     <row r="10">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>263</v>
@@ -593,7 +593,7 @@
         <v>0.380228136882129</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.380228136882129</v>
       </c>
     </row>
     <row r="11">
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
         <v>257</v>
@@ -613,7 +613,7 @@
         <v>0.389105058365759</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>0.778210116731518</v>
       </c>
     </row>
     <row r="12">
@@ -624,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
         <v>296</v>
@@ -633,7 +633,7 @@
         <v>0.675675675675676</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1.01351351351351</v>
       </c>
     </row>
     <row r="13">
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
         <v>331</v>
@@ -653,7 +653,7 @@
         <v>0.906344410876133</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.906344410876133</v>
       </c>
     </row>
     <row r="14">
@@ -664,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>371</v>
@@ -673,7 +673,7 @@
         <v>1.07816711590297</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1.07816711590297</v>
       </c>
     </row>
   </sheetData>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>58</v>
@@ -825,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1.72413793103448</v>
       </c>
     </row>
     <row r="7">
@@ -862,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
         <v>45</v>
@@ -871,7 +871,7 @@
         <v>4.44444444444444</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>4.44444444444444</v>
       </c>
     </row>
     <row r="9">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>41</v>
@@ -894,7 +894,7 @@
         <v>2.4390243902439</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>2.4390243902439</v>
       </c>
     </row>
     <row r="10">
@@ -931,7 +931,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
         <v>32</v>
@@ -940,7 +940,7 @@
         <v>12.5</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="12">
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
         <v>601</v>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.998336106489185</v>
+        <v>1.66389351081531</v>
       </c>
     </row>
     <row r="3">
@@ -1083,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
         <v>533</v>
@@ -1092,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.562851782363977</v>
+        <v>1.68855534709193</v>
       </c>
     </row>
     <row r="4">
@@ -1106,7 +1106,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E4" t="n">
         <v>516</v>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.968992248062015</v>
+        <v>3.10077519379845</v>
       </c>
     </row>
     <row r="5">
@@ -1129,7 +1129,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
         <v>500</v>
@@ -1138,7 +1138,7 @@
         <v>0.4</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -1152,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
         <v>501</v>
@@ -1161,7 +1161,7 @@
         <v>0.598802395209581</v>
       </c>
       <c r="G6" t="n">
-        <v>0.798403193612774</v>
+        <v>3.79241516966068</v>
       </c>
     </row>
     <row r="7">
@@ -1175,7 +1175,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="E7" t="n">
         <v>449</v>
@@ -1184,7 +1184,7 @@
         <v>4.23162583518931</v>
       </c>
       <c r="G7" t="n">
-        <v>0.89086859688196</v>
+        <v>6.90423162583519</v>
       </c>
     </row>
     <row r="8">
@@ -1198,7 +1198,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="E8" t="n">
         <v>443</v>
@@ -1207,7 +1207,7 @@
         <v>3.83747178329571</v>
       </c>
       <c r="G8" t="n">
-        <v>0.677200902934537</v>
+        <v>9.48081264108352</v>
       </c>
     </row>
     <row r="9">
@@ -1221,7 +1221,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E9" t="n">
         <v>421</v>
@@ -1230,7 +1230,7 @@
         <v>5.46318289786223</v>
       </c>
       <c r="G9" t="n">
-        <v>0.950118764845606</v>
+        <v>5.93824228028503</v>
       </c>
     </row>
     <row r="10">
@@ -1244,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E10" t="n">
         <v>383</v>
@@ -1253,7 +1253,7 @@
         <v>1.56657963446475</v>
       </c>
       <c r="G10" t="n">
-        <v>0.522193211488251</v>
+        <v>3.1331592689295</v>
       </c>
     </row>
     <row r="11">
@@ -1267,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E11" t="n">
         <v>372</v>
@@ -1276,7 +1276,7 @@
         <v>4.03225806451613</v>
       </c>
       <c r="G11" t="n">
-        <v>0.537634408602151</v>
+        <v>4.56989247311828</v>
       </c>
     </row>
     <row r="12">
@@ -1290,7 +1290,7 @@
         <v>65</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="E12" t="n">
         <v>334</v>
@@ -1299,7 +1299,7 @@
         <v>19.4610778443114</v>
       </c>
       <c r="G12" t="n">
-        <v>0.598802395209581</v>
+        <v>20.9580838323353</v>
       </c>
     </row>
     <row r="13">
@@ -1313,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E13" t="n">
         <v>282</v>
@@ -1322,7 +1322,7 @@
         <v>3.90070921985816</v>
       </c>
       <c r="G13" t="n">
-        <v>0.709219858156028</v>
+        <v>4.60992907801418</v>
       </c>
     </row>
     <row r="14">
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>269</v>
@@ -1345,7 +1345,7 @@
         <v>0.371747211895911</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.371747211895911</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1419,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>84</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1.19047619047619</v>
       </c>
     </row>
     <row r="4">
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>93</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>2.1505376344086</v>
       </c>
     </row>
     <row r="5">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>95</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1.05263157894737</v>
       </c>
     </row>
     <row r="6">
@@ -1488,7 +1488,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
         <v>96</v>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.04166666666667</v>
+        <v>3.125</v>
       </c>
     </row>
     <row r="7">
@@ -1511,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>89</v>
@@ -1520,7 +1520,7 @@
         <v>3.37078651685393</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>3.37078651685393</v>
       </c>
     </row>
     <row r="8">
@@ -1534,7 +1534,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
         <v>66</v>
@@ -1543,7 +1543,7 @@
         <v>3.03030303030303</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>4.54545454545455</v>
       </c>
     </row>
     <row r="9">
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>58</v>
@@ -1566,7 +1566,7 @@
         <v>1.72413793103448</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1.72413793103448</v>
       </c>
     </row>
     <row r="10">
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>56</v>
@@ -1612,7 +1612,7 @@
         <v>3.57142857142857</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>3.57142857142857</v>
       </c>
     </row>
     <row r="12">
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>34</v>
@@ -1635,7 +1635,7 @@
         <v>2.94117647058824</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>2.94117647058824</v>
       </c>
     </row>
     <row r="13">
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>235</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.70212765957447</v>
+        <v>2.12765957446809</v>
       </c>
     </row>
     <row r="3">
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
         <v>236</v>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2.96610169491525</v>
+        <v>5.50847457627119</v>
       </c>
     </row>
     <row r="6">
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>226</v>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>5.30973451327434</v>
+        <v>6.19469026548673</v>
       </c>
     </row>
     <row r="7">
@@ -1826,7 +1826,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D7" t="n">
         <v>152</v>
@@ -1835,7 +1835,7 @@
         <v>19.0789473684211</v>
       </c>
       <c r="F7" t="n">
-        <v>2.63157894736842</v>
+        <v>22.3684210526316</v>
       </c>
     </row>
     <row r="8">
@@ -1846,7 +1846,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D8" t="n">
         <v>104</v>
@@ -1855,7 +1855,7 @@
         <v>9.61538461538462</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="9">
@@ -1866,7 +1866,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
         <v>109</v>
@@ -1875,7 +1875,7 @@
         <v>2.75229357798165</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>3.6697247706422</v>
       </c>
     </row>
     <row r="10">
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
         <v>111</v>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.900900900900901</v>
+        <v>4.5045045045045</v>
       </c>
     </row>
     <row r="11">
@@ -1906,7 +1906,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
         <v>124</v>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1.61290322580645</v>
       </c>
     </row>
     <row r="12">
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
         <v>134</v>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.746268656716418</v>
       </c>
     </row>
     <row r="14">
@@ -2020,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
         <v>399</v>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>2.00501253132832</v>
+        <v>2.25563909774436</v>
       </c>
     </row>
     <row r="3">
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>380</v>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.526315789473684</v>
+        <v>1.31578947368421</v>
       </c>
     </row>
     <row r="4">
@@ -2080,7 +2080,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>474</v>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.421940928270042</v>
+        <v>0.843881856540084</v>
       </c>
     </row>
     <row r="6">
@@ -2100,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>469</v>
@@ -2109,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.426439232409382</v>
+        <v>0.852878464818763</v>
       </c>
     </row>
     <row r="7">
@@ -2120,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>477</v>
@@ -2129,7 +2129,7 @@
         <v>0.419287211740042</v>
       </c>
       <c r="F7" t="n">
-        <v>0.209643605870021</v>
+        <v>1.0482180293501</v>
       </c>
     </row>
     <row r="8">
@@ -2140,7 +2140,7 @@
         <v>95</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="D8" t="n">
         <v>332</v>
@@ -2149,7 +2149,7 @@
         <v>28.6144578313253</v>
       </c>
       <c r="F8" t="n">
-        <v>0.602409638554217</v>
+        <v>30.1204819277108</v>
       </c>
     </row>
     <row r="9">
@@ -2160,7 +2160,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>303</v>
@@ -2169,7 +2169,7 @@
         <v>2.64026402640264</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>2.97029702970297</v>
       </c>
     </row>
     <row r="10">
@@ -2180,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
         <v>258</v>
@@ -2189,7 +2189,7 @@
         <v>0.387596899224806</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1.55038759689922</v>
       </c>
     </row>
     <row r="11">
@@ -2200,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D11" t="n">
         <v>269</v>
@@ -2209,7 +2209,7 @@
         <v>4.08921933085502</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>5.94795539033457</v>
       </c>
     </row>
     <row r="12">
@@ -2220,7 +2220,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n">
         <v>273</v>
@@ -2229,7 +2229,7 @@
         <v>2.93040293040293</v>
       </c>
       <c r="F12" t="n">
-        <v>0.366300366300366</v>
+        <v>4.76190476190476</v>
       </c>
     </row>
     <row r="13">
@@ -2240,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
         <v>261</v>
@@ -2249,7 +2249,7 @@
         <v>1.53256704980843</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>2.68199233716475</v>
       </c>
     </row>
     <row r="14">
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
         <v>267</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.374531835205993</v>
+        <v>1.12359550561798</v>
       </c>
     </row>
   </sheetData>
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>745</v>
@@ -2323,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.134228187919463</v>
+        <v>0.268456375838926</v>
       </c>
     </row>
     <row r="3">
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>732</v>
@@ -2343,7 +2343,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.546448087431694</v>
+        <v>0.683060109289617</v>
       </c>
     </row>
     <row r="4">
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
         <v>813</v>
@@ -2363,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2.0910209102091</v>
+        <v>2.460024600246</v>
       </c>
     </row>
     <row r="5">
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
         <v>796</v>
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.13065326633166</v>
+        <v>1.63316582914573</v>
       </c>
     </row>
     <row r="6">
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
         <v>747</v>
@@ -2403,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.937081659973226</v>
+        <v>1.20481927710843</v>
       </c>
     </row>
     <row r="7">
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>689</v>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.145137880986938</v>
+        <v>0.58055152394775</v>
       </c>
     </row>
     <row r="8">
@@ -2434,7 +2434,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
         <v>678</v>
@@ -2443,7 +2443,7 @@
         <v>1.47492625368732</v>
       </c>
       <c r="F8" t="n">
-        <v>0.294985250737463</v>
+        <v>2.50737463126844</v>
       </c>
     </row>
     <row r="9">
@@ -2454,7 +2454,7 @@
         <v>58</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="D9" t="n">
         <v>589</v>
@@ -2463,7 +2463,7 @@
         <v>9.8471986417657</v>
       </c>
       <c r="F9" t="n">
-        <v>0.169779286926995</v>
+        <v>12.5636672325976</v>
       </c>
     </row>
     <row r="10">
@@ -2474,7 +2474,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D10" t="n">
         <v>379</v>
@@ -2483,7 +2483,7 @@
         <v>3.43007915567282</v>
       </c>
       <c r="F10" t="n">
-        <v>0.263852242744063</v>
+        <v>4.74934036939314</v>
       </c>
     </row>
     <row r="11">
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D11" t="n">
         <v>372</v>
@@ -2503,7 +2503,7 @@
         <v>5.91397849462366</v>
       </c>
       <c r="F11" t="n">
-        <v>0.806451612903226</v>
+        <v>8.60215053763441</v>
       </c>
     </row>
     <row r="12">
@@ -2514,7 +2514,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D12" t="n">
         <v>365</v>
@@ -2523,7 +2523,7 @@
         <v>1.64383561643836</v>
       </c>
       <c r="F12" t="n">
-        <v>0.273972602739726</v>
+        <v>3.56164383561644</v>
       </c>
     </row>
     <row r="13">
@@ -2534,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
         <v>355</v>
@@ -2543,7 +2543,7 @@
         <v>0.845070422535211</v>
       </c>
       <c r="F13" t="n">
-        <v>0.28169014084507</v>
+        <v>1.97183098591549</v>
       </c>
     </row>
     <row r="14">
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
         <v>344</v>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.290697674418605</v>
+        <v>0.581395348837209</v>
       </c>
     </row>
   </sheetData>
@@ -2608,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D2" t="n">
         <v>619</v>
@@ -2617,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.969305331179321</v>
+        <v>2.58481421647819</v>
       </c>
     </row>
     <row r="3">
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" t="n">
         <v>564</v>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.77304964539007</v>
+        <v>2.4822695035461</v>
       </c>
     </row>
     <row r="4">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>486</v>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.64609053497942</v>
+        <v>1.85185185185185</v>
       </c>
     </row>
     <row r="5">
@@ -2668,7 +2668,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
         <v>494</v>
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.21457489878543</v>
+        <v>2.63157894736842</v>
       </c>
     </row>
     <row r="6">
@@ -2688,7 +2688,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="n">
         <v>504</v>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2.18253968253968</v>
+        <v>2.38095238095238</v>
       </c>
     </row>
     <row r="7">
@@ -2708,7 +2708,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
         <v>473</v>
@@ -2717,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1.26849894291755</v>
+        <v>1.47991543340381</v>
       </c>
     </row>
     <row r="8">
@@ -2728,7 +2728,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
         <v>514</v>
@@ -2737,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>5.6420233463035</v>
+        <v>6.80933852140078</v>
       </c>
     </row>
     <row r="9">
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>458</v>
@@ -2757,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.436681222707424</v>
+        <v>1.96506550218341</v>
       </c>
     </row>
     <row r="10">
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D10" t="n">
         <v>452</v>
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1.54867256637168</v>
+        <v>3.09734513274336</v>
       </c>
     </row>
     <row r="11">
@@ -2788,7 +2788,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D11" t="n">
         <v>465</v>
@@ -2797,7 +2797,7 @@
         <v>4.51612903225806</v>
       </c>
       <c r="F11" t="n">
-        <v>0.21505376344086</v>
+        <v>5.80645161290323</v>
       </c>
     </row>
     <row r="12">
@@ -2808,7 +2808,7 @@
         <v>108</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="D12" t="n">
         <v>277</v>
@@ -2817,7 +2817,7 @@
         <v>38.9891696750903</v>
       </c>
       <c r="F12" t="n">
-        <v>0.36101083032491</v>
+        <v>39.3501805054152</v>
       </c>
     </row>
     <row r="13">
@@ -2828,7 +2828,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D13" t="n">
         <v>205</v>
@@ -2837,7 +2837,7 @@
         <v>7.31707317073171</v>
       </c>
       <c r="F13" t="n">
-        <v>0.48780487804878</v>
+        <v>8.29268292682927</v>
       </c>
     </row>
     <row r="14">
@@ -2848,7 +2848,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
         <v>208</v>
@@ -2857,7 +2857,7 @@
         <v>0.961538461538462</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>2.88461538461538</v>
       </c>
     </row>
   </sheetData>
@@ -2908,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>222</v>
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.45045045045045</v>
       </c>
     </row>
     <row r="3">
@@ -2931,7 +2931,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
         <v>229</v>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1.74672489082969</v>
       </c>
     </row>
     <row r="4">
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>289</v>
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03806228373702</v>
+        <v>1.3840830449827</v>
       </c>
     </row>
     <row r="5">
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
         <v>249</v>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.401606425702811</v>
+        <v>0.803212851405622</v>
       </c>
     </row>
     <row r="7">
@@ -3023,7 +3023,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>251</v>
@@ -3032,7 +3032,7 @@
         <v>0.796812749003984</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>0.796812749003984</v>
       </c>
     </row>
     <row r="8">
@@ -3046,7 +3046,7 @@
         <v>29</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E8" t="n">
         <v>190</v>
@@ -3055,7 +3055,7 @@
         <v>15.2631578947368</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>16.8421052631579</v>
       </c>
     </row>
     <row r="9">
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
         <v>156</v>
@@ -3078,7 +3078,7 @@
         <v>6.41025641025641</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>6.41025641025641</v>
       </c>
     </row>
     <row r="10">
@@ -3092,7 +3092,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
         <v>93</v>
@@ -3101,7 +3101,7 @@
         <v>2.1505376344086</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>2.1505376344086</v>
       </c>
     </row>
     <row r="11">
@@ -3115,7 +3115,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>87</v>
@@ -3124,7 +3124,7 @@
         <v>5.74712643678161</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>5.74712643678161</v>
       </c>
     </row>
     <row r="12">
@@ -3138,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
         <v>64</v>
@@ -3147,7 +3147,7 @@
         <v>6.25</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="13">
@@ -3359,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>49</v>
@@ -3368,7 +3368,7 @@
         <v>2.04081632653061</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>2.04081632653061</v>
       </c>
     </row>
     <row r="8">
@@ -3382,7 +3382,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
         <v>31</v>
@@ -3391,7 +3391,7 @@
         <v>16.1290322580645</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>16.1290322580645</v>
       </c>
     </row>
     <row r="9">
@@ -3405,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
         <v>25</v>
@@ -3414,7 +3414,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -3451,7 +3451,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>26</v>
@@ -3460,7 +3460,7 @@
         <v>3.84615384615385</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>3.84615384615385</v>
       </c>
     </row>
     <row r="12">
@@ -3626,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
         <v>215</v>
@@ -3635,7 +3635,7 @@
         <v>0.930232558139535</v>
       </c>
       <c r="G4" t="n">
-        <v>2.7906976744186</v>
+        <v>3.25581395348837</v>
       </c>
     </row>
     <row r="5">
@@ -3649,7 +3649,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
         <v>208</v>
@@ -3658,7 +3658,7 @@
         <v>2.40384615384615</v>
       </c>
       <c r="G5" t="n">
-        <v>2.88461538461538</v>
+        <v>3.36538461538462</v>
       </c>
     </row>
     <row r="6">
@@ -3695,7 +3695,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>129</v>
@@ -3704,7 +3704,7 @@
         <v>2.32558139534884</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>2.32558139534884</v>
       </c>
     </row>
     <row r="8">
@@ -3718,7 +3718,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
         <v>99</v>
@@ -3727,7 +3727,7 @@
         <v>15.1515151515152</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>16.1616161616162</v>
       </c>
     </row>
     <row r="9">
@@ -3741,7 +3741,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
         <v>64</v>
@@ -3750,7 +3750,7 @@
         <v>3.125</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>3.125</v>
       </c>
     </row>
     <row r="10">
@@ -3916,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
         <v>1073</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.65237651444548</v>
+        <v>0.745573159366263</v>
       </c>
     </row>
     <row r="3">
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" t="n">
         <v>1123</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.267141585040071</v>
+        <v>0.534283170080142</v>
       </c>
     </row>
     <row r="4">
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
         <v>1163</v>
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.60189165950129</v>
+        <v>0.945829750644884</v>
       </c>
     </row>
     <row r="5">
@@ -4008,7 +4008,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E6" t="n">
         <v>1058</v>
@@ -4017,7 +4017,7 @@
         <v>3.11909262759924</v>
       </c>
       <c r="G6" t="n">
-        <v>3.40264650283554</v>
+        <v>4.15879017013232</v>
       </c>
     </row>
     <row r="7">
@@ -4031,7 +4031,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n">
         <v>993</v>
@@ -4040,7 +4040,7 @@
         <v>1.81268882175227</v>
       </c>
       <c r="G7" t="n">
-        <v>1.4098690835851</v>
+        <v>1.91339375629406</v>
       </c>
     </row>
     <row r="8">
@@ -4054,7 +4054,7 @@
         <v>57</v>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E8" t="n">
         <v>988</v>
@@ -4063,7 +4063,7 @@
         <v>5.76923076923077</v>
       </c>
       <c r="G8" t="n">
-        <v>1.01214574898785</v>
+        <v>6.07287449392713</v>
       </c>
     </row>
     <row r="9">
@@ -4077,7 +4077,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E9" t="n">
         <v>948</v>
@@ -4086,7 +4086,7 @@
         <v>3.69198312236287</v>
       </c>
       <c r="G9" t="n">
-        <v>0.527426160337553</v>
+        <v>3.79746835443038</v>
       </c>
     </row>
     <row r="10">
@@ -4100,7 +4100,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
         <v>854</v>
@@ -4109,7 +4109,7 @@
         <v>0.819672131147541</v>
       </c>
       <c r="G10" t="n">
-        <v>0.234192037470726</v>
+        <v>1.17096018735363</v>
       </c>
     </row>
     <row r="11">
@@ -4123,7 +4123,7 @@
         <v>28</v>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E11" t="n">
         <v>875</v>
@@ -4132,7 +4132,7 @@
         <v>3.2</v>
       </c>
       <c r="G11" t="n">
-        <v>0.342857142857143</v>
+        <v>3.42857142857143</v>
       </c>
     </row>
     <row r="12">
@@ -4146,7 +4146,7 @@
         <v>54</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="E12" t="n">
         <v>800</v>
@@ -4155,7 +4155,7 @@
         <v>6.75</v>
       </c>
       <c r="G12" t="n">
-        <v>0.25</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="13">
@@ -4169,7 +4169,7 @@
         <v>14</v>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
         <v>804</v>
@@ -4178,7 +4178,7 @@
         <v>1.74129353233831</v>
       </c>
       <c r="G13" t="n">
-        <v>0.373134328358209</v>
+        <v>1.74129353233831</v>
       </c>
     </row>
     <row r="14">
@@ -4192,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
         <v>849</v>
@@ -4201,7 +4201,7 @@
         <v>0.588928150765607</v>
       </c>
       <c r="G14" t="n">
-        <v>0.588928150765607</v>
+        <v>0.706713780918728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>